<commit_message>
manual analysis for 50 github projects
</commit_message>
<xml_diff>
--- a/RQ1_Manual_Analysis_Purpose_And_Features_Of_Docker.xlsx
+++ b/RQ1_Manual_Analysis_Purpose_And_Features_Of_Docker.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Thesis\CPS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715B6EAC-EA3D-4BD0-ADED-5CD326A50CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - RQ1_Manual_Analysis_P" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - RQ1_Manual_Analysis_P" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="162">
   <si>
     <t>RQ1_Manual_Analysis_Purpose_And_Features_Of_Docker</t>
   </si>
@@ -27,7 +36,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -38,7 +47,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -49,18 +58,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://github.com/bytecodealliance/wasm-micro-runtime</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -71,7 +69,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -82,7 +80,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -93,7 +91,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -104,7 +102,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -115,7 +113,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -126,7 +124,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -137,18 +135,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://github.com/nerves-project/nerves</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -159,7 +146,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -170,7 +157,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -181,7 +168,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -192,7 +179,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -203,18 +190,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://github.com/MTASZTAKI/ApertusVR</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -225,7 +201,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -236,7 +212,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -247,7 +223,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -258,7 +234,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -269,7 +245,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -280,7 +256,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -291,7 +267,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -302,7 +278,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -313,7 +289,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -324,7 +300,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -335,7 +311,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -346,18 +322,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://github.com/hatem-darweesh/assuremappingtools</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -368,7 +333,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -379,7 +344,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -390,7 +355,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -401,7 +366,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -412,7 +377,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -423,7 +388,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -434,7 +399,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -445,7 +410,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -456,7 +421,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -467,7 +432,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -478,7 +443,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -489,7 +454,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -500,7 +465,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -511,7 +476,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -522,7 +487,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -533,7 +498,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -544,7 +509,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -555,7 +520,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -566,7 +531,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -577,7 +542,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -588,7 +553,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -599,7 +564,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -610,7 +575,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -621,7 +586,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -632,7 +597,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -643,7 +608,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -654,7 +619,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -665,7 +630,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -676,7 +641,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -687,7 +652,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -698,7 +663,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -709,7 +674,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -720,7 +685,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -731,7 +696,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -742,7 +707,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -753,7 +718,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -764,7 +729,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -775,7 +740,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -786,7 +751,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -797,7 +762,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -808,7 +773,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -819,7 +784,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -830,7 +795,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -841,7 +806,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -852,7 +817,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -863,7 +828,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -874,7 +839,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -885,7 +850,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -896,7 +861,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -907,7 +872,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -918,7 +883,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -929,7 +894,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -940,7 +905,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -951,7 +916,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -962,7 +927,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -973,7 +938,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -984,7 +949,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -995,7 +960,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -1006,7 +971,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -1017,7 +982,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -1028,7 +993,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -1039,7 +1004,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -1050,7 +1015,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -1061,7 +1026,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -1072,7 +1037,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -1083,7 +1048,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -1094,23 +1059,217 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://github.com/ucla-mobility/OpenCDA</t>
     </r>
+  </si>
+  <si>
+    <t>Targeting multiple cross platform support</t>
+  </si>
+  <si>
+    <t>creating normal build</t>
+  </si>
+  <si>
+    <t>Used Ubuntu based environment and sets up development environment.(CI)</t>
+  </si>
+  <si>
+    <t>https://github.com/nerves-project/nerves</t>
+  </si>
+  <si>
+    <t>Docker file is not used instead used a Shell script.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">using script and makefile to make builds </t>
+  </si>
+  <si>
+    <t>Docker file is not used instead it used kured-1.15.0-dockerhub.yaml file which deploys kubernetes reboot Daemon to cluster.</t>
+  </si>
+  <si>
+    <t>Automate node reboots in a Kubernetes cluster</t>
+  </si>
+  <si>
+    <t>Used two docker file
+1) DB - Environment system setup, create builds and cleanup, creates Volume and has CI
+2) Slate - create buildsCI and step by step build environment</t>
+  </si>
+  <si>
+    <t>Environment setup + running script for iniital database setup</t>
+  </si>
+  <si>
+    <t>Step by step builds and CI</t>
+  </si>
+  <si>
+    <t>Creates a containerized SSH automation tool, also has CI</t>
+  </si>
+  <si>
+    <t>caches workspace files between builds to reduce build times.</t>
+  </si>
+  <si>
+    <t>updates the CA certificates copies SSL certificates and the pre-built binary into a scratch-based container, then sets the binary as the entrypoint.</t>
+  </si>
+  <si>
+    <t>No docker file found</t>
+  </si>
+  <si>
+    <t>Using nginix in debug mode</t>
+  </si>
+  <si>
+    <t>running nginx as non-root user</t>
+  </si>
+  <si>
+    <t>install CA certificate</t>
+  </si>
+  <si>
+    <t>Environment setup for multiplatorm 1) Android and 2) Debian. Have used two dockerfile. Creating the builds</t>
+  </si>
+  <si>
+    <t>has multiple dockerfiles (most of them copy the bin and exe to local machine on docker image)</t>
+  </si>
+  <si>
+    <t>Installing packages and creating directory</t>
+  </si>
+  <si>
+    <t>Did not use dockerfile directly instead used script. This script runs a Docker container.</t>
+  </si>
+  <si>
+    <t>CI and step by step run builds</t>
+  </si>
+  <si>
+    <t>No docker file used instead used shell script (the script docker_base.sh is used for environment setup +CI)</t>
+  </si>
+  <si>
+    <t>Environment setup, install dependencies,builds, clones the project from github.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Install dependencies,builds, copy folder from local to docker image. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">running application with Jupyter Notebook and Tensorflow. Used 8887,8888 ports. </t>
+  </si>
+  <si>
+    <t>Environment setup for development(devel) and prebuilt stages. Clean the cache files</t>
+  </si>
+  <si>
+    <t>Used two docker files 
+1) base - Environment setup, create builds and storing in temperoray folder
+2) pre-built stage - Environment setup
+One script - build.sh runs both of these docker files.</t>
+  </si>
+  <si>
+    <t>https://github.com/hatem-darweesh/assuremappingtools</t>
+  </si>
+  <si>
+    <t>Environment setup, install dependencies,builds also has CUDA drivers</t>
+  </si>
+  <si>
+    <t>Install Angular dependency and use port 4200</t>
+  </si>
+  <si>
+    <t>https://github.com/bytecodealliance/wasm-micro-runtime</t>
+  </si>
+  <si>
+    <t>Step by step install packages,builds, install WebAssembly SDK(emsdk,wasi-sdk,binaryen,wabt,..) all these are downloaded using ecternal websites</t>
+  </si>
+  <si>
+    <t>layered run and creating volume.</t>
+  </si>
+  <si>
+    <t>Install dependencies and Testing</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>There are 3 docker files. 1) Tasks they do are Environment setup 2) build and runs test 3)Checks if the files are up-to-date.</t>
+  </si>
+  <si>
+    <t>Step by step installation of packages and builds, environment setup which support multiple programming lanuages. It also has CI.</t>
+  </si>
+  <si>
+    <t>creates development environment, install dependencies and use script to create builds for GCC,NrfSdk, McuBoot.</t>
+  </si>
+  <si>
+    <t>Use to patch the Go library in base image of Go environment.</t>
+  </si>
+  <si>
+    <t>CI and step by step build environment and install dependencies</t>
+  </si>
+  <si>
+    <t>create environment ready for javascript development in VSCode. clone and install emsdk.</t>
+  </si>
+  <si>
+    <t>build environment, install dependices and cleanup</t>
+  </si>
+  <si>
+    <t>multiple cross platfrom development environment( GCC,Clang, MinGW) and finally clean up of pervious builds.</t>
+  </si>
+  <si>
+    <t>Environment setup with proper memory management. Installing builds for multiple languages.</t>
+  </si>
+  <si>
+    <t>Installing packages, dependencies, cloning some of the github repo and running scripts</t>
+  </si>
+  <si>
+    <t>https://github.com/MTASZTAKI/ApertusVR</t>
+  </si>
+  <si>
+    <t>normal build</t>
+  </si>
+  <si>
+    <t>Step by step environment step, create builds, install dependencies, used some cleanup scripts, running and finally deploying.</t>
+  </si>
+  <si>
+    <t>creates a directory and runs scons</t>
+  </si>
+  <si>
+    <t>dockerfile is not used instead of it used shell scripts.</t>
+  </si>
+  <si>
+    <t>running docker and creating volumne</t>
+  </si>
+  <si>
+    <t>environment setup and creating builds, dependencies and some cleanup of pervious build folders.</t>
+  </si>
+  <si>
+    <t>created user and install dependencies step by step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">created new user, changed its permission and role, finally installed the dependencies </t>
+  </si>
+  <si>
+    <t>setup and manage the Docker container with GPU if available. Handles the region specific support and prepare runtime environment for Apollo.</t>
+  </si>
+  <si>
+    <t>Cleanup, install system packages and python dependencies.</t>
+  </si>
+  <si>
+    <t>install build, cleanup and minimize image size</t>
+  </si>
+  <si>
+    <t>installing dependencies and deploying image</t>
+  </si>
+  <si>
+    <t>create user, install dependencies and environment setup</t>
+  </si>
+  <si>
+    <t>multi-stage Docker image to run the LGSVL Simulator( stages are base, vulkan_loader,unzipper and Final)</t>
+  </si>
+  <si>
+    <t>making the build for mobile cross platform and simulator</t>
+  </si>
+  <si>
+    <t>install dependencies step by step, use port 5900 for VNC , unzip and cleanup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1122,15 +1281,26 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -1268,73 +1438,142 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -1533,7 +1772,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1551,7 +1790,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1580,7 +1819,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1605,7 +1844,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1630,7 +1869,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1655,7 +1894,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1680,7 +1919,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1705,7 +1944,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1730,7 +1969,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1755,7 +1994,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1780,7 +2019,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1793,9 +2032,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1812,7 +2057,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1830,7 +2075,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1855,7 +2100,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1880,7 +2125,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1905,7 +2150,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1930,7 +2175,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1955,7 +2200,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1980,7 +2225,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2005,7 +2250,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2030,7 +2275,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2055,7 +2300,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2068,9 +2313,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -2084,7 +2335,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2102,7 +2353,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2131,7 +2382,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2156,7 +2407,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2181,7 +2432,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2206,7 +2457,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2231,7 +2482,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2256,7 +2507,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2281,7 +2532,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2306,7 +2557,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2331,7 +2582,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2344,1255 +2595,1385 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:G101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="71.0547" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.8516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.9922" style="1" customWidth="1"/>
-    <col min="4" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="71" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44" style="1" customWidth="1"/>
+    <col min="4" max="8" width="16.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="27.6" customHeight="1">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" ht="20.25" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.25" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="8">
+      <c r="B3" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="8">
+      <c r="B4" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="8">
+      <c r="B6" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="8">
+      <c r="B7" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="8">
+      <c r="B8" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="8">
+      <c r="B9" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="8">
+      <c r="B10" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="8">
+      <c r="B11" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="8">
+      <c r="B12" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="8">
+      <c r="B14" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="8">
+      <c r="B15" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="8">
+      <c r="B16" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="8">
+      <c r="B17" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="8">
+      <c r="B18" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="8">
+      <c r="B20" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="8">
+      <c r="B21" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="8">
+      <c r="B22" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="8">
+      <c r="B23" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="8">
+      <c r="B24" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="8">
+      <c r="B25" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="8">
+      <c r="B26" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" t="s" s="8">
+      <c r="B27" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" t="s" s="8">
+      <c r="B28" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A29" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" t="s" s="8">
+      <c r="B29" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A30" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" t="s" s="8">
+      <c r="B30" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" t="s" s="8">
+      <c r="B31" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+    </row>
+    <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A33" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-    </row>
-    <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" t="s" s="8">
+      <c r="B33" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A34" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" t="s" s="8">
+      <c r="B34" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" t="s" s="8">
+      <c r="B35" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+    </row>
+    <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A36" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" t="s" s="8">
+      <c r="B36" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+    </row>
+    <row r="37" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A37" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" ht="20.05" customHeight="1">
-      <c r="A34" t="s" s="8">
+      <c r="B37" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+    </row>
+    <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A38" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+    </row>
+    <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A39" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" ht="20.05" customHeight="1">
-      <c r="A35" t="s" s="8">
+      <c r="B39" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+    </row>
+    <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A40" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" ht="20.05" customHeight="1">
-      <c r="A36" t="s" s="8">
+      <c r="B40" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+    </row>
+    <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A41" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-    </row>
-    <row r="37" ht="20.05" customHeight="1">
-      <c r="A37" t="s" s="8">
+      <c r="B41" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+    </row>
+    <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A42" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-    </row>
-    <row r="38" ht="20.05" customHeight="1">
-      <c r="A38" t="s" s="8">
-        <v>30</v>
-      </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-    </row>
-    <row r="39" ht="20.05" customHeight="1">
-      <c r="A39" t="s" s="8">
+      <c r="B42" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+    </row>
+    <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A43" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" ht="20.05" customHeight="1">
-      <c r="A40" t="s" s="8">
+      <c r="B43" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+    </row>
+    <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A44" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-    </row>
-    <row r="41" ht="20.05" customHeight="1">
-      <c r="A41" t="s" s="8">
+      <c r="B44" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+    </row>
+    <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A45" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-    </row>
-    <row r="42" ht="20.05" customHeight="1">
-      <c r="A42" t="s" s="8">
+      <c r="B45" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+    </row>
+    <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A46" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-    </row>
-    <row r="43" ht="20.05" customHeight="1">
-      <c r="A43" t="s" s="8">
+      <c r="B46" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+    </row>
+    <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A47" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-    </row>
-    <row r="44" ht="20.05" customHeight="1">
-      <c r="A44" t="s" s="8">
+      <c r="B47" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+    </row>
+    <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A48" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-    </row>
-    <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" t="s" s="8">
+      <c r="B48" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="49" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A49" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-    </row>
-    <row r="46" ht="20.05" customHeight="1">
-      <c r="A46" t="s" s="8">
+      <c r="B49" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+    </row>
+    <row r="50" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A50" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-    </row>
-    <row r="47" ht="20.05" customHeight="1">
-      <c r="A47" t="s" s="8">
+      <c r="B50" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+    </row>
+    <row r="51" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A51" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-    </row>
-    <row r="48" ht="20.05" customHeight="1">
-      <c r="A48" t="s" s="8">
+      <c r="B51" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+    </row>
+    <row r="52" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A52" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-    </row>
-    <row r="49" ht="20.05" customHeight="1">
-      <c r="A49" t="s" s="8">
+      <c r="B52" s="8"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+    </row>
+    <row r="53" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A53" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-    </row>
-    <row r="50" ht="20.05" customHeight="1">
-      <c r="A50" t="s" s="8">
+      <c r="B53" s="8"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+    </row>
+    <row r="54" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A54" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-    </row>
-    <row r="51" ht="20.05" customHeight="1">
-      <c r="A51" t="s" s="8">
+      <c r="B54" s="8"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+    </row>
+    <row r="55" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A55" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-    </row>
-    <row r="52" ht="20.05" customHeight="1">
-      <c r="A52" t="s" s="8">
+      <c r="B55" s="8"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+    </row>
+    <row r="56" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A56" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-    </row>
-    <row r="53" ht="20.05" customHeight="1">
-      <c r="A53" t="s" s="8">
+      <c r="B56" s="8"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+    </row>
+    <row r="57" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A57" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-    </row>
-    <row r="54" ht="20.05" customHeight="1">
-      <c r="A54" t="s" s="8">
+      <c r="B57" s="8"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+    </row>
+    <row r="58" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A58" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-    </row>
-    <row r="55" ht="20.05" customHeight="1">
-      <c r="A55" t="s" s="8">
+      <c r="B58" s="8"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+    </row>
+    <row r="59" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A59" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-    </row>
-    <row r="56" ht="20.05" customHeight="1">
-      <c r="A56" t="s" s="8">
+      <c r="B59" s="8"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+    </row>
+    <row r="60" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A60" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-    </row>
-    <row r="57" ht="20.05" customHeight="1">
-      <c r="A57" t="s" s="8">
+      <c r="B60" s="8"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+    </row>
+    <row r="61" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A61" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
-    </row>
-    <row r="58" ht="20.05" customHeight="1">
-      <c r="A58" t="s" s="8">
+      <c r="B61" s="8"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+    </row>
+    <row r="62" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A62" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-    </row>
-    <row r="59" ht="20.05" customHeight="1">
-      <c r="A59" t="s" s="8">
+      <c r="B62" s="8"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+    </row>
+    <row r="63" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A63" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
-    </row>
-    <row r="60" ht="20.05" customHeight="1">
-      <c r="A60" t="s" s="8">
+      <c r="B63" s="8"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+    </row>
+    <row r="64" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A64" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
-    </row>
-    <row r="61" ht="20.05" customHeight="1">
-      <c r="A61" t="s" s="8">
+      <c r="B64" s="8"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+    </row>
+    <row r="65" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A65" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
-    </row>
-    <row r="62" ht="20.05" customHeight="1">
-      <c r="A62" t="s" s="8">
+      <c r="B65" s="8"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+    </row>
+    <row r="66" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A66" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="9"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
-    </row>
-    <row r="63" ht="20.05" customHeight="1">
-      <c r="A63" t="s" s="8">
+      <c r="B66" s="8"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+    </row>
+    <row r="67" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A67" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="9"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
-    </row>
-    <row r="64" ht="20.05" customHeight="1">
-      <c r="A64" t="s" s="8">
+      <c r="B67" s="8"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+    </row>
+    <row r="68" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A68" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="9"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-    </row>
-    <row r="65" ht="20.05" customHeight="1">
-      <c r="A65" t="s" s="8">
+      <c r="B68" s="8"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+    </row>
+    <row r="69" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A69" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="9"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="10"/>
-    </row>
-    <row r="66" ht="20.05" customHeight="1">
-      <c r="A66" t="s" s="8">
+      <c r="B69" s="8"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+    </row>
+    <row r="70" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A70" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="9"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="10"/>
-    </row>
-    <row r="67" ht="20.05" customHeight="1">
-      <c r="A67" t="s" s="8">
+      <c r="B70" s="8"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+    </row>
+    <row r="71" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A71" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="9"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
-    </row>
-    <row r="68" ht="20.05" customHeight="1">
-      <c r="A68" t="s" s="8">
+      <c r="B71" s="8"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+    </row>
+    <row r="72" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A72" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="9"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="10"/>
-    </row>
-    <row r="69" ht="20.05" customHeight="1">
-      <c r="A69" t="s" s="8">
+      <c r="B72" s="8"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+    </row>
+    <row r="73" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A73" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="9"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="10"/>
-    </row>
-    <row r="70" ht="20.05" customHeight="1">
-      <c r="A70" t="s" s="8">
+      <c r="B73" s="8"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+    </row>
+    <row r="74" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A74" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="9"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
-    </row>
-    <row r="71" ht="20.05" customHeight="1">
-      <c r="A71" t="s" s="8">
+      <c r="B74" s="8"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+    </row>
+    <row r="75" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A75" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="9"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="10"/>
-    </row>
-    <row r="72" ht="20.05" customHeight="1">
-      <c r="A72" t="s" s="8">
+      <c r="B75" s="8"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+    </row>
+    <row r="76" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A76" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="9"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="10"/>
-      <c r="G72" s="10"/>
-    </row>
-    <row r="73" ht="20.05" customHeight="1">
-      <c r="A73" t="s" s="8">
+      <c r="B76" s="8"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+    </row>
+    <row r="77" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A77" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
-    </row>
-    <row r="74" ht="20.05" customHeight="1">
-      <c r="A74" t="s" s="8">
+      <c r="B77" s="8"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+    </row>
+    <row r="78" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A78" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="9"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="10"/>
-      <c r="G74" s="10"/>
-    </row>
-    <row r="75" ht="20.05" customHeight="1">
-      <c r="A75" t="s" s="8">
+      <c r="B78" s="8"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+    </row>
+    <row r="79" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A79" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="9"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="10"/>
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
-    </row>
-    <row r="76" ht="20.05" customHeight="1">
-      <c r="A76" t="s" s="8">
+      <c r="B79" s="8"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+    </row>
+    <row r="80" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A80" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="9"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
-    </row>
-    <row r="77" ht="20.05" customHeight="1">
-      <c r="A77" t="s" s="8">
+      <c r="B80" s="8"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+    </row>
+    <row r="81" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A81" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B77" s="9"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
-    </row>
-    <row r="78" ht="20.05" customHeight="1">
-      <c r="A78" t="s" s="8">
+      <c r="B81" s="8"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+    </row>
+    <row r="82" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A82" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="9"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="10"/>
-    </row>
-    <row r="79" ht="20.05" customHeight="1">
-      <c r="A79" t="s" s="8">
+      <c r="B82" s="8"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+    </row>
+    <row r="83" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A83" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="9"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="10"/>
-    </row>
-    <row r="80" ht="20.05" customHeight="1">
-      <c r="A80" t="s" s="8">
+      <c r="B83" s="8"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+    </row>
+    <row r="84" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A84" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="9"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="10"/>
-      <c r="G80" s="10"/>
-    </row>
-    <row r="81" ht="20.05" customHeight="1">
-      <c r="A81" t="s" s="8">
+      <c r="B84" s="8"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+    </row>
+    <row r="85" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A85" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="9"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="10"/>
-      <c r="G81" s="10"/>
-    </row>
-    <row r="82" ht="20.05" customHeight="1">
-      <c r="A82" t="s" s="8">
+      <c r="B85" s="8"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+    </row>
+    <row r="86" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A86" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="9"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="10"/>
-      <c r="G82" s="10"/>
-    </row>
-    <row r="83" ht="20.05" customHeight="1">
-      <c r="A83" t="s" s="8">
+      <c r="B86" s="8"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+    </row>
+    <row r="87" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A87" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B83" s="9"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="10"/>
-      <c r="F83" s="10"/>
-      <c r="G83" s="10"/>
-    </row>
-    <row r="84" ht="20.05" customHeight="1">
-      <c r="A84" t="s" s="8">
+      <c r="B87" s="8"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+    </row>
+    <row r="88" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A88" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="9"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="10"/>
-      <c r="F84" s="10"/>
-      <c r="G84" s="10"/>
-    </row>
-    <row r="85" ht="20.05" customHeight="1">
-      <c r="A85" t="s" s="8">
+      <c r="B88" s="8"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+    </row>
+    <row r="89" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A89" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="9"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="10"/>
-    </row>
-    <row r="86" ht="20.05" customHeight="1">
-      <c r="A86" t="s" s="8">
+      <c r="B89" s="8"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+    </row>
+    <row r="90" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A90" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B86" s="9"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="10"/>
-      <c r="G86" s="10"/>
-    </row>
-    <row r="87" ht="20.05" customHeight="1">
-      <c r="A87" t="s" s="8">
+      <c r="B90" s="8"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+    </row>
+    <row r="91" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A91" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B87" s="9"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="10"/>
-      <c r="F87" s="10"/>
-      <c r="G87" s="10"/>
-    </row>
-    <row r="88" ht="20.05" customHeight="1">
-      <c r="A88" t="s" s="8">
+      <c r="B91" s="8"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+    </row>
+    <row r="92" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A92" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B88" s="9"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="10"/>
-      <c r="F88" s="10"/>
-      <c r="G88" s="10"/>
-    </row>
-    <row r="89" ht="20.05" customHeight="1">
-      <c r="A89" t="s" s="8">
+      <c r="B92" s="8"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+    </row>
+    <row r="93" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A93" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B89" s="9"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="E89" s="10"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="10"/>
-    </row>
-    <row r="90" ht="20.05" customHeight="1">
-      <c r="A90" t="s" s="8">
+      <c r="B93" s="8"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+    </row>
+    <row r="94" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A94" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B90" s="9"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="10"/>
-    </row>
-    <row r="91" ht="20.05" customHeight="1">
-      <c r="A91" t="s" s="8">
+      <c r="B94" s="8"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+    </row>
+    <row r="95" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A95" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B91" s="9"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-      <c r="E91" s="10"/>
-      <c r="F91" s="10"/>
-      <c r="G91" s="10"/>
-    </row>
-    <row r="92" ht="20.05" customHeight="1">
-      <c r="A92" t="s" s="8">
+      <c r="B95" s="8"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+    </row>
+    <row r="96" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A96" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B92" s="9"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="10"/>
-    </row>
-    <row r="93" ht="20.05" customHeight="1">
-      <c r="A93" t="s" s="8">
+      <c r="B96" s="8"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="9"/>
+    </row>
+    <row r="97" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A97" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="9"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
-      <c r="E93" s="10"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="10"/>
-    </row>
-    <row r="94" ht="20.05" customHeight="1">
-      <c r="A94" t="s" s="8">
+      <c r="B97" s="8"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="9"/>
+    </row>
+    <row r="98" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A98" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="9"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="10"/>
-    </row>
-    <row r="95" ht="20.05" customHeight="1">
-      <c r="A95" t="s" s="8">
+      <c r="B98" s="8"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="9"/>
+    </row>
+    <row r="99" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A99" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B95" s="9"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10"/>
-      <c r="E95" s="10"/>
-      <c r="F95" s="10"/>
-      <c r="G95" s="10"/>
-    </row>
-    <row r="96" ht="20.05" customHeight="1">
-      <c r="A96" t="s" s="8">
+      <c r="B99" s="8"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="9"/>
+    </row>
+    <row r="100" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A100" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B96" s="9"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="10"/>
-    </row>
-    <row r="97" ht="20.05" customHeight="1">
-      <c r="A97" t="s" s="8">
+      <c r="B100" s="8"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="9"/>
+    </row>
+    <row r="101" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A101" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B97" s="9"/>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10"/>
-      <c r="F97" s="10"/>
-      <c r="G97" s="10"/>
-    </row>
-    <row r="98" ht="20.05" customHeight="1">
-      <c r="A98" t="s" s="8">
-        <v>98</v>
-      </c>
-      <c r="B98" s="9"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10"/>
-      <c r="F98" s="10"/>
-      <c r="G98" s="10"/>
-    </row>
-    <row r="99" ht="20.05" customHeight="1">
-      <c r="A99" t="s" s="8">
-        <v>99</v>
-      </c>
-      <c r="B99" s="9"/>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-      <c r="E99" s="10"/>
-      <c r="F99" s="10"/>
-      <c r="G99" s="10"/>
-    </row>
-    <row r="100" ht="20.05" customHeight="1">
-      <c r="A100" t="s" s="8">
-        <v>100</v>
-      </c>
-      <c r="B100" s="9"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="10"/>
-      <c r="F100" s="10"/>
-      <c r="G100" s="10"/>
-    </row>
-    <row r="101" ht="20.05" customHeight="1">
-      <c r="A101" t="s" s="8">
-        <v>101</v>
-      </c>
-      <c r="B101" s="9"/>
-      <c r="C101" s="10"/>
-      <c r="D101" s="10"/>
-      <c r="E101" s="10"/>
-      <c r="F101" s="10"/>
-      <c r="G101" s="10"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" location="" tooltip="" display="https://github.com/PaddlePaddle/Paddle-Lite"/>
-    <hyperlink ref="A4" r:id="rId2" location="" tooltip="" display="https://github.com/bblanchon/ArduinoJson"/>
-    <hyperlink ref="A5" r:id="rId3" location="" tooltip="" display="https://github.com/bytecodealliance/wasm-micro-runtime"/>
-    <hyperlink ref="A6" r:id="rId4" location="" tooltip="" display="https://github.com/nanopb/nanopb"/>
-    <hyperlink ref="A7" r:id="rId5" location="" tooltip="" display="https://github.com/openthread/openthread"/>
-    <hyperlink ref="A8" r:id="rId6" location="" tooltip="" display="https://github.com/microsoft/devicescript"/>
-    <hyperlink ref="A9" r:id="rId7" location="" tooltip="" display="https://github.com/apache/nuttx"/>
-    <hyperlink ref="A10" r:id="rId8" location="" tooltip="" display="https://github.com/InfiniTimeOrg/InfiniTime"/>
-    <hyperlink ref="A11" r:id="rId9" location="" tooltip="" display="https://github.com/u-root/u-root"/>
-    <hyperlink ref="A12" r:id="rId10" location="" tooltip="" display="https://github.com/LibreELEC/LibreELEC.tv"/>
-    <hyperlink ref="A13" r:id="rId11" location="" tooltip="" display="https://github.com/nerves-project/nerves"/>
-    <hyperlink ref="A14" r:id="rId12" location="" tooltip="" display="https://github.com/uTensor/uTensor"/>
-    <hyperlink ref="A15" r:id="rId13" location="" tooltip="" display="https://github.com/Luos-io/luos_engine"/>
-    <hyperlink ref="A16" r:id="rId14" location="" tooltip="" display="https://github.com/modelica/ModelicaStandardLibrary"/>
-    <hyperlink ref="A17" r:id="rId15" location="" tooltip="" display="https://github.com/INTO-CPS-Association/DTaaS"/>
-    <hyperlink ref="A18" r:id="rId16" location="" tooltip="" display="https://github.com/verivital/nnv"/>
-    <hyperlink ref="A19" r:id="rId17" location="" tooltip="" display="https://github.com/MTASZTAKI/ApertusVR"/>
-    <hyperlink ref="A20" r:id="rId18" location="" tooltip="" display="https://github.com/autowarefoundation/autoware"/>
-    <hyperlink ref="A21" r:id="rId19" location="" tooltip="" display="https://github.com/commaai/openpilot"/>
-    <hyperlink ref="A22" r:id="rId20" location="" tooltip="" display="https://github.com/gtarobotics/self-driving-car"/>
-    <hyperlink ref="A23" r:id="rId21" location="" tooltip="" display="https://github.com/microsoft/AirSim"/>
-    <hyperlink ref="A24" r:id="rId22" location="" tooltip="" display="https://github.com/lgsvl/simulator"/>
-    <hyperlink ref="A25" r:id="rId23" location="" tooltip="" display="https://github.com/erdos-project/pylot"/>
-    <hyperlink ref="A26" r:id="rId24" location="" tooltip="" display="https://github.com/Fields2Cover/Fields2Cover"/>
-    <hyperlink ref="A27" r:id="rId25" location="" tooltip="" display="https://github.com/ruhyadi/YOLO3D"/>
-    <hyperlink ref="A28" r:id="rId26" location="" tooltip="" display="https://github.com/w111liang222/lidar-slam-detection"/>
-    <hyperlink ref="A29" r:id="rId27" location="" tooltip="" display="https://github.com/ApolloAuto/apollo"/>
-    <hyperlink ref="A30" r:id="rId28" location="" tooltip="" display="https://github.com/trust-ai/SafeBench"/>
-    <hyperlink ref="A31" r:id="rId29" location="" tooltip="" display="https://github.com/truevisionai/designer"/>
-    <hyperlink ref="A32" r:id="rId30" location="" tooltip="" display="https://github.com/hatem-darweesh/assuremappingtools"/>
-    <hyperlink ref="A33" r:id="rId31" location="" tooltip="" display="https://github.com/tier4/AutowareArchitectureProposal.proj"/>
-    <hyperlink ref="A34" r:id="rId32" location="" tooltip="" display="https://github.com/autowarefoundation/autoware_core_universe_prototype"/>
-    <hyperlink ref="A35" r:id="rId33" location="" tooltip="" display="https://github.com/autorope/donkeycar"/>
-    <hyperlink ref="A36" r:id="rId34" location="" tooltip="" display="https://github.com/sigmaai/self-driving-golf-cart"/>
-    <hyperlink ref="A37" r:id="rId35" location="" tooltip="" display="https://github.com/erdos-project/erdos"/>
-    <hyperlink ref="A38" r:id="rId36" location="" tooltip="" display="https://github.com/ApolloAuto/apollo"/>
-    <hyperlink ref="A39" r:id="rId37" location="" tooltip="" display="https://github.com/aurora-opensource/xviz"/>
-    <hyperlink ref="A40" r:id="rId38" location="" tooltip="" display="https://github.com/noshluk2/ROS2-Self-Driving-Car-AI-using-OpenCV"/>
-    <hyperlink ref="A41" r:id="rId39" location="" tooltip="" display="https://github.com/amov-lab/Prometheus"/>
-    <hyperlink ref="A42" r:id="rId40" location="" tooltip="" display="https://github.com/drone-plugins/drone-docker"/>
-    <hyperlink ref="A43" r:id="rId41" location="" tooltip="" display="https://github.com/mavlink/qgroundcontrol"/>
-    <hyperlink ref="A44" r:id="rId42" location="" tooltip="" display="https://github.com/harness/drone-cli"/>
-    <hyperlink ref="A45" r:id="rId43" location="" tooltip="" display="https://github.com/Call-for-Code/DroneAid"/>
-    <hyperlink ref="A46" r:id="rId44" location="" tooltip="" display="https://github.com/amymcgovern/pyparrot"/>
-    <hyperlink ref="A47" r:id="rId45" location="" tooltip="" display="https://github.com/meltwater/drone-cache"/>
-    <hyperlink ref="A48" r:id="rId46" location="" tooltip="" display="https://github.com/appleboy/drone-ssh"/>
-    <hyperlink ref="A49" r:id="rId47" location="" tooltip="" display="https://github.com/DroneDB/DroneDB"/>
-    <hyperlink ref="A50" r:id="rId48" location="" tooltip="" display="https://github.com/mspnp/aks-fabrikam-dronedelivery"/>
-    <hyperlink ref="A51" r:id="rId49" location="" tooltip="" display="https://github.com/OpenDroneMap/WebODM"/>
-    <hyperlink ref="A52" r:id="rId50" location="" tooltip="" display="https://github.com/drone/docs"/>
-    <hyperlink ref="A53" r:id="rId51" location="" tooltip="" display="https://github.com/ipedrazas/drone-helm"/>
-    <hyperlink ref="A54" r:id="rId52" location="" tooltip="" display="https://github.com/orig74/DroneSimLab"/>
-    <hyperlink ref="A55" r:id="rId53" location="" tooltip="" display="https://github.com/OpenDroneMap/ODM"/>
-    <hyperlink ref="A56" r:id="rId54" location="" tooltip="" display="https://github.com/drone-runners/drone-runner-docker"/>
-    <hyperlink ref="A57" r:id="rId55" location="" tooltip="" display="https://github.com/microsoft/AirSim-NeurIPS2019-Drone-Racing"/>
-    <hyperlink ref="A58" r:id="rId56" location="" tooltip="" display="https://github.com/drone-runners/drone-runner-kube"/>
-    <hyperlink ref="A59" r:id="rId57" location="" tooltip="" display="https://github.com/CopterExpress/clover"/>
-    <hyperlink ref="A60" r:id="rId58" location="" tooltip="" display="https://github.com/OpenDroneMap/NodeODM"/>
-    <hyperlink ref="A61" r:id="rId59" location="" tooltip="" display="https://github.com/generalized-intelligence/GAAS"/>
-    <hyperlink ref="A62" r:id="rId60" location="" tooltip="" display="https://github.com/clydemcqueen/tello_ros"/>
-    <hyperlink ref="A63" r:id="rId61" location="" tooltip="" display="https://github.com/paparazzi/paparazzi"/>
-    <hyperlink ref="A64" r:id="rId62" location="" tooltip="" display="https://github.com/drone/charts"/>
-    <hyperlink ref="A65" r:id="rId63" location="" tooltip="" display="https://github.com/drone/drone-wall"/>
-    <hyperlink ref="A66" r:id="rId64" location="" tooltip="" display="https://github.com/DAVFoundation/missions"/>
-    <hyperlink ref="A67" r:id="rId65" location="" tooltip="" display="https://github.com/NVIDIA-AI-IOT/redtail"/>
-    <hyperlink ref="A68" r:id="rId66" location="" tooltip="" display="https://github.com/nicholasaleks/Damn-Vulnerable-Drone"/>
-    <hyperlink ref="A69" r:id="rId67" location="" tooltip="" display="https://github.com/COVESA/vsomeip"/>
-    <hyperlink ref="A70" r:id="rId68" location="" tooltip="" display="https://github.com/alexa/alexa-auto-sdk"/>
-    <hyperlink ref="A71" r:id="rId69" location="" tooltip="" display="https://github.com/Fraunhofer-AISEC/gallia"/>
-    <hyperlink ref="A72" r:id="rId70" location="" tooltip="" display="https://github.com/rusefi/rusefi"/>
-    <hyperlink ref="A73" r:id="rId71" location="" tooltip="" display="https://github.com/christoph2/pyxcp"/>
-    <hyperlink ref="A74" r:id="rId72" location="" tooltip="" display="https://github.com/vectorgrp/sil-kit"/>
-    <hyperlink ref="A75" r:id="rId73" location="" tooltip="" display="https://github.com/pylessard/python-can-isotp"/>
-    <hyperlink ref="A76" r:id="rId74" location="" tooltip="" display="https://github.com/pylessard/python-udsoncan"/>
-    <hyperlink ref="A77" r:id="rId75" location="" tooltip="" display="https://github.com/carla-simulator/carla"/>
-    <hyperlink ref="A78" r:id="rId76" location="" tooltip="" display="https://github.com/PJLab-ADG/SensorsCalibration"/>
-    <hyperlink ref="A79" r:id="rId77" location="" tooltip="" display="https://github.com/OpenDriveLab/UniAD"/>
-    <hyperlink ref="A80" r:id="rId78" location="" tooltip="" display="https://github.com/naurril/SUSTechPOINTS"/>
-    <hyperlink ref="A81" r:id="rId79" location="" tooltip="" display="https://github.com/carla-simulator/leaderboard"/>
-    <hyperlink ref="A82" r:id="rId80" location="" tooltip="" display="https://github.com/huawei-noah/SMARTS"/>
-    <hyperlink ref="A83" r:id="rId81" location="" tooltip="" display="https://github.com/awslabs/autonomous-driving-data-framework"/>
-    <hyperlink ref="A84" r:id="rId82" location="" tooltip="" display="https://github.com/autonomousvision/transfuser"/>
-    <hyperlink ref="A85" r:id="rId83" location="" tooltip="" display="https://github.com/storypku/CyberRT/tree/master"/>
-    <hyperlink ref="A86" r:id="rId84" location="" tooltip="" display="https://github.com/georghess/neurad-studio"/>
-    <hyperlink ref="A87" r:id="rId85" location="" tooltip="" display="https://github.com/tier4/CalibrationTools"/>
-    <hyperlink ref="A88" r:id="rId86" location="" tooltip="" display="https://github.com/SIAT-INVS/CarlaFLCAV"/>
-    <hyperlink ref="A89" r:id="rId87" location="" tooltip="" display="https://github.com/waymo-research/waymo-open-dataset"/>
-    <hyperlink ref="A90" r:id="rId88" location="" tooltip="" display="https://github.com/ucd-dare/CarDreamer"/>
-    <hyperlink ref="A91" r:id="rId89" location="" tooltip="" display="https://github.com/libornovax/master_thesis_code"/>
-    <hyperlink ref="A92" r:id="rId90" location="" tooltip="" display="https://github.com/PJLab-ADG/DriveArena"/>
-    <hyperlink ref="A93" r:id="rId91" location="" tooltip="" display="https://github.com/bark-simulator/bark"/>
-    <hyperlink ref="A94" r:id="rId92" location="" tooltip="" display="https://github.com/Daniel-xsy/RoboBEV"/>
-    <hyperlink ref="A95" r:id="rId93" location="" tooltip="" display="https://github.com/wangguojun2018/CenterNet3d"/>
-    <hyperlink ref="A96" r:id="rId94" location="" tooltip="" display="https://github.com/JOP-Lee/READ"/>
-    <hyperlink ref="A97" r:id="rId95" location="" tooltip="" display="https://github.com/open-mmlab/OpenPCDet"/>
-    <hyperlink ref="A98" r:id="rId96" location="" tooltip="" display="https://github.com/tusen-ai/SST"/>
-    <hyperlink ref="A99" r:id="rId97" location="" tooltip="" display="https://github.com/Kin-Zhang/mmfn"/>
-    <hyperlink ref="A100" r:id="rId98" location="" tooltip="" display="https://github.com/motional/nuplan-devkit"/>
-    <hyperlink ref="A101" r:id="rId99" location="" tooltip="" display="https://github.com/ucla-mobility/OpenCDA"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="A37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="A38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="A39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="A40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="A41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="A42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="A43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="A44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="A46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="A47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="A48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="A49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="A50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="A51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="A52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="A53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="A54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="A55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="A56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="A57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="A58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="A59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="A60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="A61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="A62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="A63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="A64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="A65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="A66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="A67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="A68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="A69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="A70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="A71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="A72" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="A73" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="A74" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="A75" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="A76" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="A77" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="A78" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="A79" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="A80" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="A81" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="A82" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="A83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="A84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="A85" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="A86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="A87" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="A88" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="A89" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="A90" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="A91" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="A92" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="A93" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="A94" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="A95" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="A96" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="A97" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="A98" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="A99" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="A100" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="A101" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
   </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Manual Analysis done for all the repos
</commit_message>
<xml_diff>
--- a/RQ1_Manual_Analysis_Purpose_And_Features_Of_Docker.xlsx
+++ b/RQ1_Manual_Analysis_Purpose_And_Features_Of_Docker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Thesis\CPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715B6EAC-EA3D-4BD0-ADED-5CD326A50CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EB5F65-6252-4550-9BB0-986ECBE07CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - RQ1_Manual_Analysis_P" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="214">
   <si>
     <t>RQ1_Manual_Analysis_Purpose_And_Features_Of_Docker</t>
   </si>
@@ -459,17 +459,6 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>https://github.com/amymcgovern/pyparrot</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
       <t>https://github.com/meltwater/drone-cache</t>
     </r>
   </si>
@@ -481,17 +470,6 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>https://github.com/appleboy/drone-ssh</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
       <t>https://github.com/DroneDB/DroneDB</t>
     </r>
   </si>
@@ -724,17 +702,6 @@
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://github.com/alexa/alexa-auto-sdk</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://github.com/Fraunhofer-AISEC/gallia</t>
     </r>
   </si>
   <si>
@@ -1100,9 +1067,6 @@
     <t>Environment setup + running script for iniital database setup</t>
   </si>
   <si>
-    <t>Step by step builds and CI</t>
-  </si>
-  <si>
     <t>Creates a containerized SSH automation tool, also has CI</t>
   </si>
   <si>
@@ -1110,9 +1074,6 @@
   </si>
   <si>
     <t>updates the CA certificates copies SSL certificates and the pre-built binary into a scratch-based container, then sets the binary as the entrypoint.</t>
-  </si>
-  <si>
-    <t>No docker file found</t>
   </si>
   <si>
     <t>Using nginix in debug mode</t>
@@ -1263,6 +1224,189 @@
   </si>
   <si>
     <t>install dependencies step by step, use port 5900 for VNC , unzip and cleanup</t>
+  </si>
+  <si>
+    <t>local build</t>
+  </si>
+  <si>
+    <t>Step by step builds</t>
+  </si>
+  <si>
+    <t>https://github.com/appleboy/drone-ssh</t>
+  </si>
+  <si>
+    <t>used port 1000 and deployed</t>
+  </si>
+  <si>
+    <t>No Dockcerfile present only the readme file are present which has mentioned about CI and CD.</t>
+  </si>
+  <si>
+    <t>Environment setup, Multi stage run (builder, final)</t>
+  </si>
+  <si>
+    <t>Step by step builds, Adding user, running some scripts</t>
+  </si>
+  <si>
+    <t>5 docker files present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setting environment variables, cleaning build, installing and running build </t>
+  </si>
+  <si>
+    <t>different docker file for different Operarting System(linux, windows)</t>
+  </si>
+  <si>
+    <t>download a tar file from website, and add ca-certificate</t>
+  </si>
+  <si>
+    <t>Install dependencies</t>
+  </si>
+  <si>
+    <t>Install dependencies, add User</t>
+  </si>
+  <si>
+    <t>Add ca-certificates and create build</t>
+  </si>
+  <si>
+    <t>No Dockerfile present only readme file is present. In readme file only docker run commnad is given.</t>
+  </si>
+  <si>
+    <t>Install dependencies and create build</t>
+  </si>
+  <si>
+    <t>Install dependencies and download some git repo</t>
+  </si>
+  <si>
+    <t>3 dockerfiles are present 
+1) dep - environment setup, install dependencies
+2) dev - install dependencies, add user, cleanup builds
+3) ci - CI</t>
+  </si>
+  <si>
+    <t>No dockerfile present. Yaml file are present.</t>
+  </si>
+  <si>
+    <t>Use port 80 and copy build to folder.</t>
+  </si>
+  <si>
+    <t>install dependencies and run</t>
+  </si>
+  <si>
+    <t>port used is 3333</t>
+  </si>
+  <si>
+    <t>port used are 14556,14557</t>
+  </si>
+  <si>
+    <t>Environment setup, step by step build and install dependencies.</t>
+  </si>
+  <si>
+    <t>install dependencies</t>
+  </si>
+  <si>
+    <t>2 dockerfiles are present 
+1) aac-ubuntu-focal -&gt; install dependencies
+2) aac-ubuntu-bionic -&gt; install dependencies</t>
+  </si>
+  <si>
+    <t>https://github.com/Fraunhofer-AISEC/gallia</t>
+  </si>
+  <si>
+    <t>install dependencies and add user</t>
+  </si>
+  <si>
+    <t>install dependencies and create build. Used CI</t>
+  </si>
+  <si>
+    <t>step by step installation of dependencies by removing pervoius python version.</t>
+  </si>
+  <si>
+    <t>install dependencies for different python versions. Used CI</t>
+  </si>
+  <si>
+    <t>install dependencies and create user</t>
+  </si>
+  <si>
+    <t>No Dockerfile is present instead script is used to bring docker up.</t>
+  </si>
+  <si>
+    <t>Step by step install dependencies and create builds, environment setup</t>
+  </si>
+  <si>
+    <t>used port 8081</t>
+  </si>
+  <si>
+    <t>install dependencies and run the project using run.sh script</t>
+  </si>
+  <si>
+    <t>There are 2 docker files.</t>
+  </si>
+  <si>
+    <t>There are 13 docker files.</t>
+  </si>
+  <si>
+    <t>Step by step install dependencies and create builds, environment setup, create user, run scripts</t>
+  </si>
+  <si>
+    <t>No dockerfile present only readme file is present.</t>
+  </si>
+  <si>
+    <t>install dependencies and environment setup.</t>
+  </si>
+  <si>
+    <t>install dependencies and cleanup</t>
+  </si>
+  <si>
+    <t>step by step install dependencies and build</t>
+  </si>
+  <si>
+    <t>step by step install dependencies and build, running scripts</t>
+  </si>
+  <si>
+    <t>scripts used are install-dmlab.sh, install-atari.sh, install-minecraft.sh</t>
+  </si>
+  <si>
+    <t>(2 dockerfiles) used for CPU and GPU</t>
+  </si>
+  <si>
+    <t>12 dockerfiles</t>
+  </si>
+  <si>
+    <t>step by step install dependencies</t>
+  </si>
+  <si>
+    <t>step by step install dependencies and environment setup</t>
+  </si>
+  <si>
+    <t>2 dockerfiles are present</t>
+  </si>
+  <si>
+    <t>2 dockerfiles are present 
+1) CI -&gt; install dependencies, environment setup and CI
+2) install dependencies, run scripts</t>
+  </si>
+  <si>
+    <t>there are 3 dockerfile</t>
+  </si>
+  <si>
+    <t>install dependencies and install conda environment from website links.</t>
+  </si>
+  <si>
+    <t>environment setup, install dependencies.</t>
+  </si>
+  <si>
+    <t>step by step install dependencies, add user and environment setup</t>
+  </si>
+  <si>
+    <t>5 dockerfiles are present 
+1) qgc -&gt; environment setup, install ca certificates, create user and groups, install dependencies, run scripts.
+2) simulator -&gt; environment setup, step by step installing dependencies and builds, cleanup, ports used are 8000,8080,9002
+3) flight-controller -&gt; environment setup, step by step installing dependencies and builds, create user and groups, running scripts, ports used are 5760, 9003.
+4) companion-computer -&gt; environment setup, step by step installing dependencies and builds, create SSH server, run script, ports used are 3000, 5000, 22.
+5) ground-control-station -&gt; install dependencies</t>
+  </si>
+  <si>
+    <t>5 docker files present, docker-compose.yaml is used to run all these dockerfiles.</t>
   </si>
 </sst>
 </file>
@@ -1477,14 +1621,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2616,9 +2760,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
@@ -2631,15 +2775,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.6" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -2661,10 +2805,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2676,23 +2820,25 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="9"/>
+        <v>96</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>157</v>
+      </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="11" t="s">
-        <v>130</v>
+      <c r="A5" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -2704,10 +2850,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -2719,7 +2865,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -2732,7 +2878,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -2745,7 +2891,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -2758,7 +2904,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -2771,7 +2917,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -2784,10 +2930,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -2795,14 +2941,14 @@
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="11" t="s">
-        <v>101</v>
+      <c r="A13" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -2814,7 +2960,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -2827,7 +2973,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -2840,7 +2986,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -2853,7 +2999,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -2866,7 +3012,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -2875,11 +3021,11 @@
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="11" t="s">
-        <v>145</v>
+      <c r="A19" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -2892,7 +3038,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -2905,7 +3051,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -2918,10 +3064,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -2933,7 +3079,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2945,8 +3091,8 @@
       <c r="A24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>159</v>
+      <c r="B24" s="11" t="s">
+        <v>154</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -2959,7 +3105,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -2972,7 +3118,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -2985,7 +3131,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -2998,7 +3144,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -3011,10 +3157,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>154</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -3026,10 +3172,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -3041,7 +3187,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -3050,11 +3196,11 @@
       <c r="G31" s="9"/>
     </row>
     <row r="32" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="11" t="s">
-        <v>127</v>
+      <c r="A32" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -3067,7 +3213,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -3080,7 +3226,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -3093,7 +3239,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -3106,7 +3252,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -3119,7 +3265,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
@@ -3132,7 +3278,7 @@
         <v>27</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
@@ -3145,7 +3291,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -3158,7 +3304,7 @@
         <v>36</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
@@ -3171,7 +3317,7 @@
         <v>37</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -3184,7 +3330,7 @@
         <v>38</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
@@ -3197,7 +3343,7 @@
         <v>39</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
@@ -3210,7 +3356,7 @@
         <v>40</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
@@ -3223,10 +3369,10 @@
         <v>41</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
@@ -3234,12 +3380,8 @@
       <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A46" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A46" s="7"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -3248,13 +3390,13 @@
     </row>
     <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -3262,13 +3404,15 @@
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A48" s="7" t="s">
-        <v>44</v>
+      <c r="A48" s="10" t="s">
+        <v>159</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C48" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>160</v>
+      </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -3276,10 +3420,10 @@
     </row>
     <row r="49" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
@@ -3289,13 +3433,13 @@
     </row>
     <row r="50" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
@@ -3304,13 +3448,13 @@
     </row>
     <row r="51" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
@@ -3319,9 +3463,11 @@
     </row>
     <row r="52" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B52" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>161</v>
+      </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
@@ -3330,9 +3476,11 @@
     </row>
     <row r="53" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B53" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>162</v>
+      </c>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
@@ -3341,10 +3489,14 @@
     </row>
     <row r="54" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>164</v>
+      </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
@@ -3352,9 +3504,11 @@
     </row>
     <row r="55" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B55" s="8"/>
+        <v>49</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>165</v>
+      </c>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
@@ -3363,10 +3517,14 @@
     </row>
     <row r="56" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="9"/>
+        <v>50</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>166</v>
+      </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
@@ -3374,9 +3532,11 @@
     </row>
     <row r="57" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
@@ -3385,9 +3545,11 @@
     </row>
     <row r="58" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B58" s="8"/>
+        <v>52</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>170</v>
+      </c>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
@@ -3396,9 +3558,11 @@
     </row>
     <row r="59" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B59" s="8"/>
+        <v>53</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>171</v>
+      </c>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
@@ -3407,9 +3571,11 @@
     </row>
     <row r="60" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" s="8"/>
+        <v>54</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>168</v>
+      </c>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
@@ -3418,9 +3584,11 @@
     </row>
     <row r="61" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B61" s="8"/>
+        <v>55</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>172</v>
+      </c>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
@@ -3429,9 +3597,11 @@
     </row>
     <row r="62" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B62" s="8"/>
+        <v>56</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>173</v>
+      </c>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
@@ -3440,9 +3610,11 @@
     </row>
     <row r="63" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B63" s="8"/>
+        <v>57</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>174</v>
+      </c>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
@@ -3451,9 +3623,11 @@
     </row>
     <row r="64" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B64" s="8"/>
+        <v>58</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>175</v>
+      </c>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
@@ -3462,9 +3636,11 @@
     </row>
     <row r="65" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B65" s="8"/>
+        <v>59</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>176</v>
+      </c>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
@@ -3473,10 +3649,14 @@
     </row>
     <row r="66" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="9"/>
+        <v>60</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>178</v>
+      </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
@@ -3484,10 +3664,14 @@
     </row>
     <row r="67" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A67" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B67" s="8"/>
-      <c r="C67" s="9"/>
+        <v>61</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
@@ -3495,10 +3679,14 @@
     </row>
     <row r="68" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A68" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>213</v>
+      </c>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
@@ -3506,9 +3694,11 @@
     </row>
     <row r="69" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>181</v>
+      </c>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
@@ -3517,9 +3707,11 @@
     </row>
     <row r="70" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B70" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
@@ -3527,10 +3719,12 @@
       <c r="G70" s="9"/>
     </row>
     <row r="71" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A71" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" s="8"/>
+      <c r="A71" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>181</v>
+      </c>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
@@ -3539,9 +3733,11 @@
     </row>
     <row r="72" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A72" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B72" s="8"/>
+        <v>65</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>184</v>
+      </c>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
@@ -3550,9 +3746,11 @@
     </row>
     <row r="73" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A73" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B73" s="8"/>
+        <v>66</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>172</v>
+      </c>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
@@ -3561,9 +3759,11 @@
     </row>
     <row r="74" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A74" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" s="8"/>
+        <v>67</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>185</v>
+      </c>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
@@ -3572,10 +3772,14 @@
     </row>
     <row r="75" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A75" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
@@ -3583,10 +3787,14 @@
     </row>
     <row r="76" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A76" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B76" s="8"/>
-      <c r="C76" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
@@ -3594,9 +3802,11 @@
     </row>
     <row r="77" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A77" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B77" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>188</v>
+      </c>
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
@@ -3605,9 +3815,11 @@
     </row>
     <row r="78" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A78" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B78" s="8"/>
+        <v>71</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>189</v>
+      </c>
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
@@ -3616,9 +3828,11 @@
     </row>
     <row r="79" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A79" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B79" s="8"/>
+        <v>72</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>190</v>
+      </c>
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
@@ -3627,10 +3841,14 @@
     </row>
     <row r="80" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A80" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B80" s="8"/>
-      <c r="C80" s="9"/>
+        <v>73</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>191</v>
+      </c>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
@@ -3638,9 +3856,11 @@
     </row>
     <row r="81" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A81" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B81" s="8"/>
+        <v>74</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>190</v>
+      </c>
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
@@ -3649,10 +3869,14 @@
     </row>
     <row r="82" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A82" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B82" s="8"/>
-      <c r="C82" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>193</v>
+      </c>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
       <c r="F82" s="9"/>
@@ -3660,10 +3884,14 @@
     </row>
     <row r="83" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A83" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B83" s="8"/>
-      <c r="C83" s="9"/>
+        <v>76</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>194</v>
+      </c>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
@@ -3671,9 +3899,11 @@
     </row>
     <row r="84" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A84" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B84" s="8"/>
+        <v>77</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>197</v>
+      </c>
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
@@ -3682,9 +3912,11 @@
     </row>
     <row r="85" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A85" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B85" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>196</v>
+      </c>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
@@ -3693,9 +3925,11 @@
     </row>
     <row r="86" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A86" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B86" s="8"/>
+        <v>79</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>197</v>
+      </c>
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
@@ -3704,9 +3938,11 @@
     </row>
     <row r="87" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A87" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B87" s="8"/>
+        <v>80</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>198</v>
+      </c>
       <c r="C87" s="9"/>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
@@ -3715,9 +3951,11 @@
     </row>
     <row r="88" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A88" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B88" s="8"/>
+        <v>81</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>199</v>
+      </c>
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
@@ -3726,9 +3964,11 @@
     </row>
     <row r="89" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A89" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B89" s="8"/>
+        <v>82</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>199</v>
+      </c>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
@@ -3737,10 +3977,14 @@
     </row>
     <row r="90" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A90" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B90" s="8"/>
-      <c r="C90" s="9"/>
+        <v>83</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>201</v>
+      </c>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
@@ -3748,10 +3992,14 @@
     </row>
     <row r="91" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A91" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B91" s="8"/>
-      <c r="C91" s="9"/>
+        <v>84</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>202</v>
+      </c>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
@@ -3759,10 +4007,14 @@
     </row>
     <row r="92" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A92" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B92" s="8"/>
-      <c r="C92" s="9"/>
+        <v>85</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
@@ -3770,10 +4022,14 @@
     </row>
     <row r="93" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A93" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B93" s="8"/>
-      <c r="C93" s="9"/>
+        <v>86</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>206</v>
+      </c>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
@@ -3781,10 +4037,14 @@
     </row>
     <row r="94" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A94" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B94" s="8"/>
-      <c r="C94" s="9"/>
+        <v>87</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>208</v>
+      </c>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
@@ -3792,9 +4052,11 @@
     </row>
     <row r="95" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A95" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B95" s="8"/>
+        <v>88</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>181</v>
+      </c>
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
@@ -3803,9 +4065,11 @@
     </row>
     <row r="96" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A96" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B96" s="8"/>
+        <v>89</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>197</v>
+      </c>
       <c r="C96" s="9"/>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
@@ -3814,9 +4078,11 @@
     </row>
     <row r="97" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A97" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B97" s="8"/>
+        <v>90</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>204</v>
+      </c>
       <c r="C97" s="9"/>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
@@ -3825,9 +4091,11 @@
     </row>
     <row r="98" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A98" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B98" s="8"/>
+        <v>91</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>181</v>
+      </c>
       <c r="C98" s="9"/>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
@@ -3836,9 +4104,11 @@
     </row>
     <row r="99" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A99" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B99" s="8"/>
+        <v>92</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>209</v>
+      </c>
       <c r="C99" s="9"/>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
@@ -3847,9 +4117,11 @@
     </row>
     <row r="100" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A100" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B100" s="8"/>
+        <v>93</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>210</v>
+      </c>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
@@ -3858,9 +4130,11 @@
     </row>
     <row r="101" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A101" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B101" s="8"/>
+        <v>94</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>211</v>
+      </c>
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
@@ -3915,62 +4189,61 @@
     <hyperlink ref="A43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
     <hyperlink ref="A44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
     <hyperlink ref="A45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="A46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="A47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="A48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="A49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="A50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="A51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="A52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="A53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="A54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="A55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="A56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="A57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="A58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="A59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="A60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="A61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="A62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="A63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="A64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="A65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="A66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="A67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="A68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="A69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="A70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="A71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="A72" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="A73" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="A74" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="A75" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="A76" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="A77" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="A78" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="A79" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="A80" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="A81" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="A82" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="A83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="A84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="A85" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="A86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="A87" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="A88" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="A89" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="A90" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="A91" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="A92" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="A93" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="A94" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="A95" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="A96" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="A97" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="A98" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="A99" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="A100" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="A101" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="A47" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="A48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="A49" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="A50" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="A51" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="A52" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="A53" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="A54" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="A55" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="A56" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="A57" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="A58" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="A59" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="A60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="A61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="A62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="A63" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="A64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="A65" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="A66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="A67" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="A68" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="A69" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="A70" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="A71" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="A72" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="A73" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="A74" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="A75" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="A76" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="A77" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="A78" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="A79" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="A80" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="A81" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="A82" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="A83" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="A84" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="A85" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="A86" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="A87" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="A88" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="A89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="A90" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="A91" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="A92" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="A93" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="A94" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="A95" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="A96" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="A97" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="A98" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="A99" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="A100" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="A101" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup scale="72" orientation="portrait"/>

</xml_diff>